<commit_message>
File cleanup + more granular specification of repo path
</commit_message>
<xml_diff>
--- a/workflow/python/output/covid_disparities_output_2020-05-08.xlsx
+++ b/workflow/python/output/covid_disparities_output_2020-05-08.xlsx
@@ -502,16 +502,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>32179</v>
+        <v>32177</v>
       </c>
       <c r="E5" t="n">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="F5" t="n">
         <v>36</v>
       </c>
       <c r="G5" t="n">
-        <v>49.61</v>
+        <v>49.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>